<commit_message>
Maj gitignore et début de liens entre maze et tilesheet
</commit_message>
<xml_diff>
--- a/doc/sceen.xlsx
+++ b/doc/sceen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Documents\Cours\L2\Archi\Labyrinthe68k\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0431BABB-55DC-434A-A617-DA5E41198447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC37761-57A7-4861-8D60-0A790757FEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3F5B3D15-AEFF-43C5-AE0B-C97CD2692EC2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F5B3D15-AEFF-43C5-AE0B-C97CD2692EC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,7 +59,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -183,6 +179,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -190,9 +192,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -509,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{635F446E-A659-4FB6-AB19-F1D3A60338CE}">
-  <dimension ref="AB10:AU24"/>
+  <dimension ref="AB9:AU24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AT22" sqref="AT22:AU23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -520,27 +519,49 @@
     <col min="1" max="16384" width="4.5703125" style="4"/>
   </cols>
   <sheetData>
+    <row r="9" spans="28:47" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="3"/>
+    </row>
     <row r="10" spans="28:47" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2"/>
-      <c r="AE10" s="2"/>
-      <c r="AF10" s="2"/>
-      <c r="AG10" s="2"/>
-      <c r="AH10" s="2"/>
-      <c r="AI10" s="2"/>
-      <c r="AJ10" s="2"/>
-      <c r="AK10" s="2"/>
-      <c r="AL10" s="2"/>
-      <c r="AM10" s="2"/>
-      <c r="AN10" s="2"/>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="2"/>
-      <c r="AQ10" s="2"/>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="2"/>
-      <c r="AT10" s="2"/>
-      <c r="AU10" s="3"/>
+      <c r="AB10" s="5"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="6"/>
+      <c r="AU10" s="7"/>
     </row>
     <row r="11" spans="28:47" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AB11" s="5"/>
@@ -661,8 +682,8 @@
       <c r="AG16" s="6"/>
       <c r="AH16" s="6"/>
       <c r="AI16" s="6"/>
-      <c r="AJ16" s="6"/>
-      <c r="AK16" s="6"/>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
       <c r="AL16" s="6"/>
       <c r="AM16" s="6"/>
       <c r="AN16" s="6"/>
@@ -683,8 +704,8 @@
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
       <c r="AI17" s="6"/>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" s="11"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
       <c r="AL17" s="6"/>
       <c r="AM17" s="6"/>
       <c r="AN17" s="6"/>
@@ -807,29 +828,29 @@
       <c r="AU22" s="7"/>
     </row>
     <row r="23" spans="28:47" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AB23" s="5"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="6"/>
-      <c r="AE23" s="6"/>
-      <c r="AF23" s="6"/>
-      <c r="AG23" s="6"/>
-      <c r="AH23" s="6"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
-      <c r="AK23" s="6"/>
-      <c r="AL23" s="6"/>
-      <c r="AM23" s="6"/>
-      <c r="AN23" s="6"/>
-      <c r="AO23" s="6"/>
-      <c r="AP23" s="6"/>
-      <c r="AQ23" s="6"/>
-      <c r="AR23" s="6"/>
-      <c r="AS23" s="6"/>
-      <c r="AT23" s="6"/>
-      <c r="AU23" s="7"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="11"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="11"/>
+      <c r="AI23" s="11"/>
+      <c r="AJ23" s="11"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="11"/>
+      <c r="AM23" s="11"/>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="11"/>
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="11"/>
+      <c r="AU23" s="12"/>
     </row>
     <row r="24" spans="28:47" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AB24" s="8"/>
+      <c r="AB24" s="9"/>
       <c r="AC24" s="9"/>
       <c r="AD24" s="9"/>
       <c r="AE24" s="9"/>
@@ -848,9 +869,81 @@
       <c r="AR24" s="9"/>
       <c r="AS24" s="9"/>
       <c r="AT24" s="9"/>
-      <c r="AU24" s="10"/>
+      <c r="AU24" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="70">
+    <mergeCell ref="AT18:AU19"/>
+    <mergeCell ref="AR18:AS19"/>
+    <mergeCell ref="AP18:AQ19"/>
+    <mergeCell ref="AN18:AO19"/>
+    <mergeCell ref="AL18:AM19"/>
+    <mergeCell ref="AJ18:AK19"/>
+    <mergeCell ref="AT20:AU21"/>
+    <mergeCell ref="AR20:AS21"/>
+    <mergeCell ref="AP20:AQ21"/>
+    <mergeCell ref="AN20:AO21"/>
+    <mergeCell ref="AL20:AM21"/>
+    <mergeCell ref="AJ20:AK21"/>
+    <mergeCell ref="AT22:AU23"/>
+    <mergeCell ref="AR22:AS23"/>
+    <mergeCell ref="AP22:AQ23"/>
+    <mergeCell ref="AN22:AO23"/>
+    <mergeCell ref="AL22:AM23"/>
+    <mergeCell ref="AJ22:AK23"/>
+    <mergeCell ref="AD22:AE23"/>
+    <mergeCell ref="AD20:AE21"/>
+    <mergeCell ref="AD18:AE19"/>
+    <mergeCell ref="AB22:AC23"/>
+    <mergeCell ref="AB20:AC21"/>
+    <mergeCell ref="AB18:AC19"/>
+    <mergeCell ref="AH22:AI23"/>
+    <mergeCell ref="AH20:AI21"/>
+    <mergeCell ref="AH18:AI19"/>
+    <mergeCell ref="AF22:AG23"/>
+    <mergeCell ref="AF20:AG21"/>
+    <mergeCell ref="AF18:AG19"/>
+    <mergeCell ref="AL14:AM15"/>
+    <mergeCell ref="AJ14:AK15"/>
+    <mergeCell ref="AH14:AI15"/>
+    <mergeCell ref="AF14:AG15"/>
+    <mergeCell ref="AD14:AE15"/>
+    <mergeCell ref="AB14:AC15"/>
+    <mergeCell ref="AN16:AO17"/>
+    <mergeCell ref="AP16:AQ17"/>
+    <mergeCell ref="AR16:AS17"/>
+    <mergeCell ref="AT16:AU17"/>
+    <mergeCell ref="AT14:AU15"/>
+    <mergeCell ref="AR14:AS15"/>
+    <mergeCell ref="AP14:AQ15"/>
+    <mergeCell ref="AN14:AO15"/>
+    <mergeCell ref="AB16:AC17"/>
+    <mergeCell ref="AD16:AE17"/>
+    <mergeCell ref="AF16:AG17"/>
+    <mergeCell ref="AH16:AI17"/>
+    <mergeCell ref="AJ16:AK17"/>
+    <mergeCell ref="AL16:AM17"/>
+    <mergeCell ref="AH12:AI13"/>
+    <mergeCell ref="AF12:AG13"/>
+    <mergeCell ref="AD12:AE13"/>
+    <mergeCell ref="AB12:AC13"/>
+    <mergeCell ref="AT10:AU11"/>
+    <mergeCell ref="AR10:AS11"/>
+    <mergeCell ref="AP10:AQ11"/>
+    <mergeCell ref="AT12:AU13"/>
+    <mergeCell ref="AR12:AS13"/>
+    <mergeCell ref="AP12:AQ13"/>
+    <mergeCell ref="AN12:AO13"/>
+    <mergeCell ref="AL12:AM13"/>
+    <mergeCell ref="AJ12:AK13"/>
+    <mergeCell ref="AB10:AC11"/>
+    <mergeCell ref="AD10:AE11"/>
+    <mergeCell ref="AF10:AG11"/>
+    <mergeCell ref="AH10:AI11"/>
+    <mergeCell ref="AN10:AO11"/>
+    <mergeCell ref="AL10:AM11"/>
+    <mergeCell ref="AJ10:AK11"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>